<commit_message>
updated risks and table
</commit_message>
<xml_diff>
--- a/risikomatrise-bachelor-oppgave.xlsx
+++ b/risikomatrise-bachelor-oppgave.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\name\Skule\2026-vaar\IDATA2901-bachelor-thesis\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\bachelor-thesis\Bachelor-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88922FE6-D2A3-440A-ABFD-38D86110261E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CED5E2C-2A7E-4E9E-8899-30184A45A888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7DA24DE4-A95E-49DB-BE50-D12AE0870C77}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="15700" xr2:uid="{7DA24DE4-A95E-49DB-BE50-D12AE0870C77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Svært sannsynlig 5</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Passe på at arbeidet følger plan og eventuelt hente inn igjen arbeidet utenom vanlig arbeids tid</t>
+  </si>
+  <si>
+    <t>Applikasjonen blir ikke det som oppdragsgiver hadde håpet på</t>
+  </si>
+  <si>
+    <t>Møter annenhver uke for å diskutere å planlegge behov for brukere</t>
+  </si>
+  <si>
+    <t>4, 8</t>
   </si>
 </sst>
 </file>
@@ -186,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -321,9 +330,20 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -331,22 +351,62 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -354,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,36 +476,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -468,6 +538,223 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>687294</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>448235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>448235</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC1B05CF-3B99-3B3B-0264-B44AC648FE7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3242235" y="2136588"/>
+          <a:ext cx="963706" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>605118</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>268941</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF668817-5B8E-8D1F-690A-148FD4686ED9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7769412" y="4938059"/>
+          <a:ext cx="0" cy="545353"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>657412</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>515470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>478117</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>418353</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11679C72-4CEC-A1EF-243F-162DBEA33764}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3212353" y="3966882"/>
+          <a:ext cx="2136588" cy="784412"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>724647</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>470647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>500529</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>403412</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB7A38BC-2F72-E99A-DDA9-8C9F064F6805}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5595471" y="3922059"/>
+          <a:ext cx="933823" cy="814294"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,31 +1074,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65294FD-C59D-4798-856C-00899A5E48C8}">
-  <dimension ref="B9:K25"/>
+  <dimension ref="B9:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="19" style="9" customWidth="1"/>
-    <col min="4" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="8" width="16.5546875" style="9" customWidth="1"/>
+    <col min="4" max="5" width="16.54296875" customWidth="1"/>
+    <col min="6" max="8" width="16.54296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="3:11" s="1" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="3:11" s="1" customFormat="1" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="D10" s="5">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6">
+        <v>7</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="3:11" s="1" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:11" s="1" customFormat="1" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="19" t="s">
         <v>1</v>
       </c>
@@ -824,7 +1115,7 @@
       <c r="H11" s="15"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="3:11" s="1" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:11" s="1" customFormat="1" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="19" t="s">
         <v>2</v>
       </c>
@@ -832,25 +1123,31 @@
         <v>1</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="12">
+        <v>6</v>
+      </c>
+      <c r="G12" s="11">
+        <v>8</v>
+      </c>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="3:11" s="1" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:11" s="1" customFormat="1" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4">
+        <v>6</v>
+      </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="13">
-        <v>4</v>
+      <c r="F13" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="3:11" s="1" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:11" s="1" customFormat="1" ht="69.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="19" t="s">
         <v>4</v>
       </c>
@@ -864,7 +1161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="20"/>
       <c r="D15" s="7" t="s">
         <v>5</v>
@@ -882,196 +1179,229 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="2:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="21"/>
-      <c r="C18" s="22" t="s">
+    <row r="18" spans="2:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="22"/>
+      <c r="C18" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="25">
+    <row r="19" spans="2:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="28">
         <v>1</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="31">
         <v>3</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="31">
         <v>1</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25">
+    <row r="20" spans="2:8" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="28">
         <v>2</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="31">
         <v>1</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="31">
         <v>3</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="25">
+    <row r="21" spans="2:8" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="28">
         <v>3</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="31">
         <v>4</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="31">
         <v>2</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="H21" s="34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="25">
+    <row r="22" spans="2:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="28">
         <v>4</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="31">
         <v>2</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="31">
         <v>3</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="25">
+    <row r="23" spans="2:8" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="28">
         <v>5</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="31">
         <v>2</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="31">
         <v>5</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="33">
         <v>1</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="34">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="25">
+    <row r="24" spans="2:8" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="28">
         <v>6</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="31">
+        <v>3</v>
+      </c>
+      <c r="E24" s="31">
+        <v>3</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="33">
+        <v>2</v>
+      </c>
+      <c r="H24" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="28">
+        <v>7</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="31">
+        <v>5</v>
+      </c>
+      <c r="E25" s="31">
+        <v>2</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="33">
+        <v>5</v>
+      </c>
+      <c r="H25" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="29">
+        <v>8</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="32">
+        <v>3</v>
+      </c>
+      <c r="E26" s="32">
         <v>4</v>
       </c>
-      <c r="E24" s="27">
+      <c r="F26" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="26">
+        <v>2</v>
+      </c>
+      <c r="H26" s="27">
         <v>3</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="26">
-        <v>4</v>
-      </c>
-      <c r="H24" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="31">
-        <v>7</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="32">
-        <v>5</v>
-      </c>
-      <c r="E25" s="32">
-        <v>2</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="29">
-        <v>5</v>
-      </c>
-      <c r="H25" s="30">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="66" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005F39A7C1C63195488FF01C4637BF8410" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdeb92a15f8633286db240a0a16a6caf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a027f5c3-149a-4c02-bec8-9aa3da99a4a6" xmlns:ns4="a2cbe04d-1bc5-4dcb-9627-1f7b95af064f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a18d4a4e28be77af03403093731ebf48" ns3:_="" ns4:_="">
     <xsd:import namespace="a027f5c3-149a-4c02-bec8-9aa3da99a4a6"/>
@@ -1292,15 +1622,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1310,6 +1631,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCF8DA-EA98-46A6-9B4B-01AA347DD578}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170A1A2C-A772-493B-8438-4EF7D1414B1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1324,14 +1653,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93DCF8DA-EA98-46A6-9B4B-01AA347DD578}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>